<commit_message>
sidebar icon navigation done
</commit_message>
<xml_diff>
--- a/Project_TimeLine_2021_4_Feb.xlsx
+++ b/Project_TimeLine_2021_4_Feb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\lms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C121E3-FA22-4EA6-969C-5E27A3AEFEE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B842CAA-27F6-4241-8C72-7272FE1CBC63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>S/N</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Front-end: Login/Signup page</t>
   </si>
   <si>
-    <t>Front-end: Dashboard</t>
-  </si>
-  <si>
     <t>Front-end: Integrate Threejs scene</t>
   </si>
   <si>
@@ -118,6 +115,15 @@
   </si>
   <si>
     <t>Front-end: Dark mode toggle</t>
+  </si>
+  <si>
+    <t>Front-end: Dashboard view</t>
+  </si>
+  <si>
+    <t>Front-end: Dashboard main page</t>
+  </si>
+  <si>
+    <t>Dashboard as a whole took longer than expected, need more time to complete the view page</t>
   </si>
 </sst>
 </file>
@@ -495,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +755,7 @@
         <v>44223</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
         <v>21</v>
@@ -760,7 +766,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -773,6 +779,12 @@
       </c>
       <c r="F11" s="3">
         <v>44230</v>
+      </c>
+      <c r="G11" s="3">
+        <v>44230</v>
+      </c>
+      <c r="I11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -780,19 +792,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3">
         <v>44231</v>
       </c>
       <c r="F12" s="3">
-        <v>44238</v>
+        <v>44237</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -800,19 +812,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E13" s="3">
-        <v>44239</v>
+        <v>44238</v>
       </c>
       <c r="F13" s="3">
-        <v>44243</v>
+        <v>44246</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -820,19 +832,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="3">
-        <v>44244</v>
+        <v>44249</v>
       </c>
       <c r="F14" s="3">
-        <v>44245</v>
+        <v>44251</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -840,7 +852,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -848,9 +860,29 @@
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="H15" t="s">
+      <c r="E15" s="3">
+        <v>44252</v>
+      </c>
+      <c r="F15" s="3">
+        <v>44253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="H16" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>